<commit_message>
Improving page and upload data
</commit_message>
<xml_diff>
--- a/code/Recipes/Recipes.xlsx
+++ b/code/Recipes/Recipes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="582">
   <si>
     <t>ID</t>
   </si>
@@ -298,9 +298,6 @@
     <t>6197cff2fce7c231035ca2e0</t>
   </si>
   <si>
-    <t>61168aaaf575165d513340b2</t>
-  </si>
-  <si>
     <t>61168ac6fabe8d0d893ce622</t>
   </si>
   <si>
@@ -1219,9 +1216,6 @@
     <t>https://www.blueapron.com/recipes/pan-seared-duck-breasts-with-crispy-duck-fat-rice-sesame-ginger-arugula-salad</t>
   </si>
   <si>
-    <t>https://www.blueapron.com/recipes/pan-seared-duck-breasts-with-crispy-duck-fat-rice-sesame-ginger-arugula-salad-3</t>
-  </si>
-  <si>
     <t>https://www.blueapron.com/recipes/wellness-meal-prep-bundle-with-chicken-salmon-4</t>
   </si>
   <si>
@@ -1264,24 +1258,15 @@
     <t>https://www.blueapron.com/recipes/spicy-beef-sesame-noodles-with-bok-choy-ede49315-31fa-40f0-a90b-6fe6c2183bef</t>
   </si>
   <si>
-    <t>https://www.blueapron.com/recipes/spicy-beef-sesame-noodles-with-bok-choy</t>
-  </si>
-  <si>
     <t>https://www.blueapron.com/recipes/tilapia-creamy-curry-sauce-with-sesame-bok-choy-rice-0ac5d768-9571-4054-b0e1-459adfd42b95</t>
   </si>
   <si>
     <t>https://www.blueapron.com/recipes/pork-chorizo-meatballs-poblano-rice-with-chipotle-peanut-sauce</t>
   </si>
   <si>
-    <t>https://www.blueapron.com/recipes/creamy-prosciutto-tomato-pasta-with-brown-butter-breadcrumbs-e762f868-4c9e-4d12-a3ed-74973b30792c</t>
-  </si>
-  <si>
     <t>https://www.blueapron.com/recipes/sheet-pan-pesto-salmon-with-a-roasted-vegetable-medley-6</t>
   </si>
   <si>
-    <t>https://www.blueapron.com/recipes/blackened-cajun-burger-with-roasted-sweet-potatoes-spicy-ketchup-3</t>
-  </si>
-  <si>
     <t>https://www.blueapron.com/recipes/miso-ponzu-beyond-burger-with-sesame-shishitos-mushrooms</t>
   </si>
   <si>
@@ -1480,15 +1465,6 @@
     <t>https://www.blueapron.com/recipes/chicken-farro-grain-bowl-with-arugula-roasted-vegetables</t>
   </si>
   <si>
-    <t>https://www.blueapron.com/recipes/surf-turf-steaks-chicken-salmon-shrimp-31</t>
-  </si>
-  <si>
-    <t>https://www.blueapron.com/recipes/specialty-selection-ny-strip-steaks-scallops-prime-ground-beef-29</t>
-  </si>
-  <si>
-    <t>https://www.blueapron.com/recipes/seafood-trio-salmon-shrimp-scallops-31</t>
-  </si>
-  <si>
     <t>https://www.blueapron.com/recipes/spicy-orange-glazed-yellowtail-fillets-with-fried-rice-candied-cashews</t>
   </si>
   <si>
@@ -1528,15 +1504,9 @@
     <t>https://www.blueapron.com/recipes/seared-steaks-mashed-potatoes-with-sauteed-carrots-homemade-steak-sauce-b618f7b2-87b8-416c-893d-5fa4c26b60c7</t>
   </si>
   <si>
-    <t>https://www.blueapron.com/recipes/basil-pesto-gnocchi-with-mushrooms-pistachio-breadcrumbs-027549ac-099a-486a-ae37-8d8956275082</t>
-  </si>
-  <si>
     <t>https://www.blueapron.com/recipes/thai-chicken-curry-peanut-noodles-with-carrots-shishito-peppers</t>
   </si>
   <si>
-    <t>https://www.blueapron.com/recipes/spicy-orange-glazed-yellowtail-fillets-with-fried-rice-candied-cashews-3</t>
-  </si>
-  <si>
     <t>https://www.blueapron.com/recipes/spicy-zucchini-quesadillas-with-poblano-pepper-fried-eggs-dc6e5fae-e73c-4ad6-a5c2-b6ae91a11488</t>
   </si>
   <si>
@@ -1561,9 +1531,6 @@
     <t>https://www.blueapron.com/recipes/crispy-garlic-herb-gnocchi-with-creamy-basil-pesto</t>
   </si>
   <si>
-    <t>https://www.blueapron.com/recipes/thai-chicken-curry-peanut-noodles-with-carrots-shishito-peppers-a83d9e72-a810-4d6b-8ead-fb90b1beea0d</t>
-  </si>
-  <si>
     <t>https://www.everyplate.com/recipes/garlic-rosemary-chicken-6197b58889cfe006315a2882</t>
   </si>
   <si>
@@ -1637,9 +1604,6 @@
   </si>
   <si>
     <t>https://www.everyplate.com/recipes/cheese-tastic-southwestern-hash-6197cff2fce7c231035ca2e0</t>
-  </si>
-  <si>
-    <t>https://www.everyplate.com/recipes/6-chicken-breasts-61168aaaf575165d513340b2</t>
   </si>
   <si>
     <t>https://www.everyplate.com/recipes/4-chicken-breasts-2-ranch-steaks-61168ac6fabe8d0d893ce622</t>
@@ -2166,7 +2130,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D230"/>
+  <dimension ref="A1:D219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2191,13 +2155,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2205,13 +2169,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D3" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2219,13 +2183,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D4" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2233,13 +2197,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D5" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2247,13 +2211,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D6" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2261,13 +2225,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D7" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2275,13 +2239,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D8" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2289,13 +2253,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D9" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2303,13 +2267,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D10" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2317,13 +2281,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D11" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2331,13 +2295,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D12" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2345,13 +2309,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D13" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2359,13 +2323,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D14" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2373,13 +2337,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D15" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2387,13 +2351,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D16" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2401,13 +2365,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D17" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2415,13 +2379,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D18" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2429,13 +2393,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D19" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2443,13 +2407,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D20" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2457,13 +2421,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D21" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2471,13 +2435,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D22" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2485,13 +2449,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D23" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2499,13 +2463,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D24" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2513,13 +2477,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D25" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2527,13 +2491,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D26" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2541,13 +2505,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D27" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2555,13 +2519,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D28" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2569,13 +2533,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D29" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2583,13 +2547,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D30" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2597,13 +2561,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D31" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2611,13 +2575,13 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D32" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2625,13 +2589,13 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D33" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2639,13 +2603,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D34" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2653,13 +2617,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D35" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2667,13 +2631,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D36" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2681,13 +2645,13 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D37" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2695,13 +2659,13 @@
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D38" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2709,57 +2673,57 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D39" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="B40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D40" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="B41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D41" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="B42" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D42" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="B43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D43" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2767,10 +2731,10 @@
         <v>182</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D44" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2778,10 +2742,10 @@
         <v>183</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D45" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2789,10 +2753,10 @@
         <v>184</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D46" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2800,10 +2764,10 @@
         <v>185</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D47" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2811,10 +2775,10 @@
         <v>186</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D48" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -2822,10 +2786,10 @@
         <v>187</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D49" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -2833,10 +2797,10 @@
         <v>188</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D50" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="51" spans="2:4">
@@ -2844,10 +2808,10 @@
         <v>189</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D51" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="52" spans="2:4">
@@ -2855,10 +2819,10 @@
         <v>190</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D52" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -2866,10 +2830,10 @@
         <v>191</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D53" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="54" spans="2:4">
@@ -2877,10 +2841,10 @@
         <v>192</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D54" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -2888,10 +2852,10 @@
         <v>193</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D55" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="56" spans="2:4">
@@ -2899,10 +2863,10 @@
         <v>194</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D56" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="57" spans="2:4">
@@ -2910,10 +2874,10 @@
         <v>195</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D57" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -2921,2199 +2885,2075 @@
         <v>196</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D58" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="B59" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D59" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="B60" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D60" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="B61" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D61" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="62" spans="2:4">
       <c r="B62" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D62" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="63" spans="2:4">
       <c r="B63" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D63" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D64" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="65" spans="2:4">
       <c r="B65" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D65" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="66" spans="2:4">
       <c r="B66" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D66" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
     </row>
     <row r="67" spans="2:4">
       <c r="B67" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D67" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
     </row>
     <row r="68" spans="2:4">
       <c r="B68" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D68" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
     </row>
     <row r="69" spans="2:4">
       <c r="B69" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D69" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="B70" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D70" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="71" spans="2:4">
       <c r="B71" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D71" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="B72" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D72" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="73" spans="2:4">
       <c r="B73" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D73" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="74" spans="2:4">
       <c r="B74" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D74" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="B75" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D75" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="76" spans="2:4">
       <c r="B76" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D76" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="77" spans="2:4">
       <c r="B77" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D77" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="78" spans="2:4">
       <c r="B78" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D78" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="79" spans="2:4">
       <c r="B79" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D79" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="80" spans="2:4">
       <c r="B80" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D80" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="81" spans="2:4">
       <c r="B81" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D81" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="82" spans="2:4">
       <c r="B82" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D82" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="83" spans="2:4">
       <c r="B83" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D83" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="84" spans="2:4">
       <c r="B84" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D84" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="85" spans="2:4">
       <c r="B85" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D85" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="86" spans="2:4">
       <c r="B86" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D86" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="87" spans="2:4">
       <c r="B87" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D87" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="88" spans="2:4">
       <c r="B88" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D88" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="89" spans="2:4">
       <c r="B89" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D89" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="90" spans="2:4">
       <c r="B90" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D90" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="91" spans="2:4">
       <c r="B91" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D91" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="B92" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D92" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="93" spans="2:4">
       <c r="B93" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D93" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="94" spans="2:4">
       <c r="B94" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D94" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="95" spans="2:4">
       <c r="B95" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D95" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="96" spans="2:4">
       <c r="B96" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D96" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="B97" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C97" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D97" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>42</v>
+      </c>
+      <c r="B98" t="s">
+        <v>236</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="D97" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="B98" t="s">
-        <v>233</v>
-      </c>
-      <c r="C98" s="2" t="s">
+      <c r="D98" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>43</v>
+      </c>
+      <c r="B99" t="s">
+        <v>237</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="D98" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="B99" t="s">
-        <v>234</v>
-      </c>
-      <c r="C99" s="2" t="s">
+      <c r="D99" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>44</v>
+      </c>
+      <c r="B100" t="s">
+        <v>238</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="D99" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="B100" t="s">
-        <v>235</v>
-      </c>
-      <c r="C100" s="2" t="s">
+      <c r="D100" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" t="s">
+        <v>45</v>
+      </c>
+      <c r="B101" t="s">
+        <v>239</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="D100" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="B101" t="s">
-        <v>236</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>458</v>
-      </c>
       <c r="D101" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B102" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D102" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B103" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D103" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B104" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D104" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B105" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D105" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B106" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D106" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B107" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D107" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B108" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D108" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B109" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D109" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B110" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D110" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B111" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D111" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D112" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B113" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D113" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B114" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D114" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B115" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D115" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B116" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D116" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B117" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D117" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B118" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D118" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B119" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D119" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B120" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D120" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B121" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D121" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B122" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D122" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B123" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D123" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B124" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C124" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="D124" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="B125" t="s">
+        <v>263</v>
+      </c>
+      <c r="C125" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="D124" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4">
-      <c r="A125" t="s">
-        <v>65</v>
-      </c>
-      <c r="B125" t="s">
-        <v>260</v>
-      </c>
-      <c r="C125" s="2" t="s">
+      <c r="D125" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="B126" t="s">
+        <v>264</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="D125" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
-      <c r="A126" t="s">
-        <v>66</v>
-      </c>
-      <c r="B126" t="s">
-        <v>261</v>
-      </c>
-      <c r="C126" s="2" t="s">
+      <c r="D126" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="B127" t="s">
+        <v>265</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="D126" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4">
-      <c r="A127" t="s">
-        <v>67</v>
-      </c>
-      <c r="B127" t="s">
-        <v>262</v>
-      </c>
-      <c r="C127" s="2" t="s">
+      <c r="D127" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="B128" t="s">
+        <v>266</v>
+      </c>
+      <c r="C128" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="D127" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4">
-      <c r="A128" t="s">
-        <v>68</v>
-      </c>
-      <c r="B128" t="s">
-        <v>263</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>485</v>
-      </c>
       <c r="D128" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
     </row>
     <row r="129" spans="2:4">
       <c r="B129" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D129" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="130" spans="2:4">
       <c r="B130" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D130" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="131" spans="2:4">
       <c r="B131" t="s">
-        <v>184</v>
+        <v>269</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D131" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="132" spans="2:4">
       <c r="B132" t="s">
-        <v>185</v>
+        <v>270</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D132" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="133" spans="2:4">
       <c r="B133" t="s">
-        <v>186</v>
+        <v>271</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D133" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="134" spans="2:4">
       <c r="B134" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D134" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="135" spans="2:4">
       <c r="B135" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D135" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="136" spans="2:4">
       <c r="B136" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D136" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="137" spans="2:4">
       <c r="B137" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D137" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="138" spans="2:4">
       <c r="B138" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D138" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="139" spans="2:4">
       <c r="B139" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D139" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="140" spans="2:4">
       <c r="B140" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D140" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="141" spans="2:4">
       <c r="B141" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D141" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="142" spans="2:4">
       <c r="B142" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D142" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="143" spans="2:4">
       <c r="B143" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D143" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="144" spans="2:4">
       <c r="B144" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D144" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="B145" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D145" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="B146" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D146" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="B147" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D147" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="B148" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="C148" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="D148" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>69</v>
+      </c>
+      <c r="B149" t="s">
+        <v>287</v>
+      </c>
+      <c r="C149" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="D148" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
-      <c r="B149" t="s">
-        <v>266</v>
-      </c>
-      <c r="C149" s="2" t="s">
+      <c r="D149" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="s">
+        <v>70</v>
+      </c>
+      <c r="B150" t="s">
+        <v>288</v>
+      </c>
+      <c r="C150" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="D149" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
-      <c r="B150" t="s">
-        <v>280</v>
-      </c>
-      <c r="C150" s="2" t="s">
+      <c r="D150" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" t="s">
+        <v>71</v>
+      </c>
+      <c r="B151" t="s">
+        <v>289</v>
+      </c>
+      <c r="C151" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="D150" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4">
-      <c r="B151" t="s">
-        <v>281</v>
-      </c>
-      <c r="C151" s="2" t="s">
+      <c r="D151" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" t="s">
+        <v>72</v>
+      </c>
+      <c r="B152" t="s">
+        <v>290</v>
+      </c>
+      <c r="C152" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="D151" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4">
-      <c r="B152" t="s">
-        <v>282</v>
-      </c>
-      <c r="C152" s="2" t="s">
+      <c r="D152" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" t="s">
+        <v>73</v>
+      </c>
+      <c r="B153" t="s">
+        <v>291</v>
+      </c>
+      <c r="C153" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="D152" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4">
-      <c r="B153" t="s">
-        <v>283</v>
-      </c>
-      <c r="C153" s="2" t="s">
+      <c r="D153" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" t="s">
+        <v>74</v>
+      </c>
+      <c r="B154" t="s">
+        <v>292</v>
+      </c>
+      <c r="C154" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="D153" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
-      <c r="B154" t="s">
-        <v>284</v>
-      </c>
-      <c r="C154" s="2" t="s">
+      <c r="D154" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" t="s">
+        <v>75</v>
+      </c>
+      <c r="B155" t="s">
+        <v>293</v>
+      </c>
+      <c r="C155" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="D154" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
-      <c r="B155" t="s">
-        <v>285</v>
-      </c>
-      <c r="C155" s="2" t="s">
+      <c r="D155" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="s">
+        <v>76</v>
+      </c>
+      <c r="B156" t="s">
+        <v>294</v>
+      </c>
+      <c r="C156" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="D155" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4">
-      <c r="B156" t="s">
-        <v>286</v>
-      </c>
-      <c r="C156" s="2" t="s">
+      <c r="D156" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" t="s">
+        <v>77</v>
+      </c>
+      <c r="B157" t="s">
+        <v>295</v>
+      </c>
+      <c r="C157" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="D156" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4">
-      <c r="B157" t="s">
-        <v>287</v>
-      </c>
-      <c r="C157" s="2" t="s">
+      <c r="D157" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" t="s">
+        <v>78</v>
+      </c>
+      <c r="B158" t="s">
+        <v>296</v>
+      </c>
+      <c r="C158" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="D157" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
-      <c r="B158" t="s">
-        <v>279</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>515</v>
-      </c>
       <c r="D158" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B159" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D159" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B160" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D160" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B161" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D161" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B162" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D162" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B163" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D163" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B164" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D164" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B165" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D165" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B166" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D166" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B167" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D167" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B168" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D168" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B169" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D169" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B170" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D170" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B171" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D171" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B172" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D172" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B173" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D173" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B174" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D174" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B175" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D175" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B176" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D176" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B177" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D177" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B178" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D178" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B179" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D179" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B180" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D180" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B181" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D181" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B182" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D182" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B183" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D183" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B184" t="s">
-        <v>262</v>
+        <v>322</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D184" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B185" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D185" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="B186" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D186" t="s">
-        <v>592</v>
+        <v>580</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B187" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D187" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B188" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D188" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B189" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D189" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B190" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D190" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B191" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D191" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B192" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D192" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B193" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D193" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="B194" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D194" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B195" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D195" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B196" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D196" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B197" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D197" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="B198" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D198" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B199" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D199" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B200" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D200" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B201" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D201" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B202" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D202" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B203" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D203" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="B204" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D204" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B205" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D205" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B206" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D206" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B207" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D207" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B208" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D208" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B209" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D209" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B210" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D210" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B211" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D211" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B212" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D212" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B213" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D213" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B214" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D214" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B215" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D215" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B216" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D216" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="B217" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D217" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B218" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D218" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B219" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D219" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4">
-      <c r="A220" t="s">
-        <v>130</v>
-      </c>
-      <c r="B220" t="s">
-        <v>348</v>
-      </c>
-      <c r="C220" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="D220" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4">
-      <c r="A221" t="s">
-        <v>131</v>
-      </c>
-      <c r="B221" t="s">
-        <v>349</v>
-      </c>
-      <c r="C221" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="D221" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4">
-      <c r="A222" t="s">
-        <v>132</v>
-      </c>
-      <c r="B222" t="s">
-        <v>350</v>
-      </c>
-      <c r="C222" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="D222" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4">
-      <c r="A223" t="s">
-        <v>133</v>
-      </c>
-      <c r="B223" t="s">
-        <v>351</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="D223" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4">
-      <c r="A224" t="s">
-        <v>134</v>
-      </c>
-      <c r="B224" t="s">
-        <v>352</v>
-      </c>
-      <c r="C224" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="D224" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4">
-      <c r="A225" t="s">
-        <v>135</v>
-      </c>
-      <c r="B225" t="s">
-        <v>353</v>
-      </c>
-      <c r="C225" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="D225" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4">
-      <c r="A226" t="s">
-        <v>136</v>
-      </c>
-      <c r="B226" t="s">
-        <v>354</v>
-      </c>
-      <c r="C226" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="D226" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4">
-      <c r="A227" t="s">
-        <v>137</v>
-      </c>
-      <c r="B227" t="s">
-        <v>355</v>
-      </c>
-      <c r="C227" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="D227" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4">
-      <c r="A228" t="s">
-        <v>138</v>
-      </c>
-      <c r="B228" t="s">
-        <v>356</v>
-      </c>
-      <c r="C228" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="D228" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4">
-      <c r="A229" t="s">
-        <v>139</v>
-      </c>
-      <c r="B229" t="s">
-        <v>357</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="D229" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4">
-      <c r="A230" t="s">
-        <v>140</v>
-      </c>
-      <c r="B230" t="s">
-        <v>358</v>
-      </c>
-      <c r="C230" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="D230" t="s">
-        <v>593</v>
       </c>
     </row>
   </sheetData>
@@ -5336,17 +5176,6 @@
     <hyperlink ref="C217" r:id="rId216"/>
     <hyperlink ref="C218" r:id="rId217"/>
     <hyperlink ref="C219" r:id="rId218"/>
-    <hyperlink ref="C220" r:id="rId219"/>
-    <hyperlink ref="C221" r:id="rId220"/>
-    <hyperlink ref="C222" r:id="rId221"/>
-    <hyperlink ref="C223" r:id="rId222"/>
-    <hyperlink ref="C224" r:id="rId223"/>
-    <hyperlink ref="C225" r:id="rId224"/>
-    <hyperlink ref="C226" r:id="rId225"/>
-    <hyperlink ref="C227" r:id="rId226"/>
-    <hyperlink ref="C228" r:id="rId227"/>
-    <hyperlink ref="C229" r:id="rId228"/>
-    <hyperlink ref="C230" r:id="rId229"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>